<commit_message>
Updates to the main code
</commit_message>
<xml_diff>
--- a/ADCS/Components Database-Real.xlsx
+++ b/ADCS/Components Database-Real.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/IcyHotFrancis/Documents/Cornell/Masters/SYSEN 5900 Research/Matlab Code/Satellite-Design-Tool/ADCS/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900" activeTab="1"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Camera" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="253">
   <si>
     <t>Camera</t>
   </si>
@@ -769,6 +774,51 @@
   </si>
   <si>
     <t>96x90x11</t>
+  </si>
+  <si>
+    <t>FireSat II Components</t>
+  </si>
+  <si>
+    <t>CMG</t>
+  </si>
+  <si>
+    <t>Sun Sensor</t>
+  </si>
+  <si>
+    <t>Star Sensor</t>
+  </si>
+  <si>
+    <t>Horizon Sensors</t>
+  </si>
+  <si>
+    <t>Horizon</t>
+  </si>
+  <si>
+    <t>Honeywell</t>
+  </si>
+  <si>
+    <t>Reaction Wheel</t>
+  </si>
+  <si>
+    <t>267x120</t>
+  </si>
+  <si>
+    <t>http://www51.honeywell.com/aero/common/documents/myaerospacecatalog-documents/HR_0610_Reaction_Wheel.pdf</t>
+  </si>
+  <si>
+    <t>http://www51.honeywell.com/aero/common/documents/myaerospacecatalog-documents/M50_Control_Moment_Gyroscope.pdf</t>
+  </si>
+  <si>
+    <t>715x200</t>
+  </si>
+  <si>
+    <t>715x200x400</t>
+  </si>
+  <si>
+    <t>Magnetorquer</t>
+  </si>
+  <si>
+    <t>Mag Sensor</t>
   </si>
 </sst>
 </file>
@@ -1026,28 +1076,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1318,7 +1368,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1332,13 +1382,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" thickBot="1">
+    <row r="1" spans="1:11" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1423,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1408,7 +1458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1443,7 +1493,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -1480,11 +1530,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1496,7 +1541,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
@@ -1504,7 +1549,7 @@
     <col min="8" max="8" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1530,7 +1575,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1601,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1582,7 +1627,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1608,7 +1653,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1636,23 +1681,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
@@ -1661,7 +1701,7 @@
     <col min="12" max="12" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="43" thickBot="1">
+    <row r="1" spans="1:15" ht="46" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1708,7 +1748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>123</v>
       </c>
@@ -1749,7 +1789,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>61</v>
       </c>
@@ -1790,7 +1830,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>56</v>
       </c>
@@ -1831,7 +1871,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>56</v>
       </c>
@@ -1872,7 +1912,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>56</v>
       </c>
@@ -1913,7 +1953,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>123</v>
       </c>
@@ -1951,7 +1991,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>123</v>
       </c>
@@ -1989,7 +2029,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>111</v>
       </c>
@@ -2027,7 +2067,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>56</v>
       </c>
@@ -2068,7 +2108,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>56</v>
       </c>
@@ -2109,7 +2149,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>192</v>
       </c>
@@ -2147,164 +2187,159 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13">
+        <v>5000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" s="6">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>829.5</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I13" s="6">
+        <v>8</v>
+      </c>
+      <c r="J13" s="6">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K13" s="6">
+        <v>6000</v>
+      </c>
+      <c r="L13" s="6">
+        <v>12</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14">
+        <v>28000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E14" s="6">
+        <v>95</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>4645.2</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I14" s="6">
+        <v>8</v>
+      </c>
+      <c r="J14" s="6">
+        <v>75</v>
+      </c>
+      <c r="K14" s="6">
+        <v>6000</v>
+      </c>
+      <c r="L14" s="6">
+        <v>75</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C15">
+        <v>50000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="6">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>8295</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I15" s="6">
+        <v>8</v>
+      </c>
+      <c r="J15" s="6">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>229</v>
+      </c>
+      <c r="N15">
+        <v>4000</v>
+      </c>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="C14">
+      <c r="C17">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>64</v>
       </c>
-      <c r="E14">
+      <c r="E17">
         <v>0.5</v>
-      </c>
-      <c r="F14">
-        <v>0.5</v>
-      </c>
-      <c r="G14">
-        <v>3.1569099999999999</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I14" s="6">
-        <v>8</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
-        <v>0</v>
-      </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" t="s">
-        <v>227</v>
-      </c>
-      <c r="O14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15">
-        <v>0.36</v>
-      </c>
-      <c r="F15">
-        <v>0.3</v>
-      </c>
-      <c r="G15">
-        <v>6.1749200000000002</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I15" s="6">
-        <v>8</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6">
-        <v>0</v>
-      </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
-        <v>227</v>
-      </c>
-      <c r="O15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16">
-        <v>0.6</v>
-      </c>
-      <c r="F16">
-        <v>0.3</v>
-      </c>
-      <c r="G16">
-        <v>9.9632199999999997</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I16" s="6">
-        <v>8</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6">
-        <v>0</v>
-      </c>
-      <c r="M16" t="s">
-        <v>227</v>
-      </c>
-      <c r="O16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17">
-        <v>6.5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17">
-        <v>0.115</v>
       </c>
       <c r="F17">
         <v>0.5</v>
       </c>
       <c r="G17">
-        <v>3.92679</v>
-      </c>
-      <c r="H17" s="17">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I17" s="17">
+        <v>3.1569099999999999</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I17" s="6">
         <v>8</v>
       </c>
       <c r="J17" s="6">
@@ -2320,35 +2355,35 @@
         <v>227</v>
       </c>
       <c r="O17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>65</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>200</v>
+        <v>66</v>
       </c>
       <c r="E18">
-        <v>0.01</v>
+        <v>0.36</v>
       </c>
       <c r="F18">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G18">
-        <v>2.3997999999999999</v>
-      </c>
-      <c r="H18" s="17">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I18" s="17">
+        <v>6.1749200000000002</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I18" s="6">
         <v>8</v>
       </c>
       <c r="J18" s="6">
@@ -2364,35 +2399,35 @@
         <v>227</v>
       </c>
       <c r="O18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>68</v>
       </c>
       <c r="C19">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
       <c r="E19">
-        <v>2.5999999999999999E-2</v>
+        <v>0.6</v>
       </c>
       <c r="F19">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G19">
-        <v>10.796989999999999</v>
-      </c>
-      <c r="H19" s="17">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I19" s="17">
+        <v>9.9632199999999997</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I19" s="6">
         <v>8</v>
       </c>
       <c r="J19" s="6">
@@ -2408,30 +2443,30 @@
         <v>227</v>
       </c>
       <c r="O19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C20">
-        <v>300</v>
+        <v>6.5</v>
       </c>
       <c r="D20" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="E20">
-        <v>0.1</v>
+        <v>0.115</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G20">
-        <v>122.8</v>
+        <v>3.92679</v>
       </c>
       <c r="H20" s="17">
         <v>0.99990000000000001</v>
@@ -2452,30 +2487,30 @@
         <v>227</v>
       </c>
       <c r="O20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C21">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E21">
-        <v>0.36</v>
+        <v>0.01</v>
       </c>
       <c r="F21">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
-        <v>4.5814399999999997</v>
+        <v>2.3997999999999999</v>
       </c>
       <c r="H21" s="17">
         <v>0.99990000000000001</v>
@@ -2493,30 +2528,33 @@
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C22">
-        <v>85</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>237</v>
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22">
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G22">
-        <v>14.2995</v>
+        <v>10.796989999999999</v>
       </c>
       <c r="H22" s="17">
         <v>0.99990000000000001</v>
@@ -2534,33 +2572,33 @@
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>116</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C23">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="D23" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E23">
-        <v>6.5</v>
+        <v>0.1</v>
       </c>
       <c r="F23">
-        <v>1.39E-3</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>354.3</v>
+        <v>122.8</v>
       </c>
       <c r="H23" s="17">
         <v>0.99990000000000001</v>
@@ -2578,33 +2616,33 @@
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="O23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C24">
-        <v>1400</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="E24">
-        <v>6.5</v>
+        <v>0.36</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="G24">
-        <v>546.20000000000005</v>
+        <v>4.5814399999999997</v>
       </c>
       <c r="H24" s="17">
         <v>0.99990000000000001</v>
@@ -2622,33 +2660,30 @@
         <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C25">
-        <v>200</v>
-      </c>
-      <c r="D25" t="s">
-        <v>211</v>
-      </c>
-      <c r="E25">
-        <v>0.7</v>
+        <v>85</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G25">
-        <v>12.113250000000001</v>
+        <v>14.2995</v>
       </c>
       <c r="H25" s="17">
         <v>0.99990000000000001</v>
@@ -2666,156 +2701,405 @@
         <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="O25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>116</v>
       </c>
       <c r="B26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26">
+        <v>1200</v>
+      </c>
+      <c r="D26" t="s">
+        <v>216</v>
+      </c>
+      <c r="E26">
+        <v>6.5</v>
+      </c>
+      <c r="F26">
+        <v>1.39E-3</v>
+      </c>
+      <c r="G26">
+        <v>354.3</v>
+      </c>
+      <c r="H26" s="17">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I26" s="17">
+        <v>8</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6">
+        <v>0</v>
+      </c>
+      <c r="L26" s="6">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>231</v>
+      </c>
+      <c r="O26" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27">
+        <v>1400</v>
+      </c>
+      <c r="D27" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27">
+        <v>6.5</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>546.20000000000005</v>
+      </c>
+      <c r="H27" s="17">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I27" s="17">
+        <v>8</v>
+      </c>
+      <c r="J27" s="6">
+        <v>0</v>
+      </c>
+      <c r="K27" s="6">
+        <v>0</v>
+      </c>
+      <c r="L27" s="6">
+        <v>0</v>
+      </c>
+      <c r="M27" t="s">
+        <v>231</v>
+      </c>
+      <c r="O27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28">
+        <v>200</v>
+      </c>
+      <c r="D28" t="s">
+        <v>211</v>
+      </c>
+      <c r="E28">
+        <v>0.7</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>12.113250000000001</v>
+      </c>
+      <c r="H28" s="17">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I28" s="17">
+        <v>8</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0</v>
+      </c>
+      <c r="L28" s="6">
+        <v>0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>252</v>
+      </c>
+      <c r="O28" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" t="s">
         <v>223</v>
       </c>
-      <c r="C26">
+      <c r="C29">
         <v>190</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>224</v>
       </c>
-      <c r="E26">
+      <c r="E29">
         <v>0.3</v>
       </c>
-      <c r="F26">
+      <c r="F29">
         <v>10</v>
       </c>
-      <c r="G26">
+      <c r="G29">
         <v>125.8</v>
       </c>
-      <c r="H26" s="17">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I26" s="17">
-        <v>8</v>
-      </c>
-      <c r="J26" s="6">
-        <v>0</v>
-      </c>
-      <c r="K26" s="6">
-        <v>0</v>
-      </c>
-      <c r="L26" s="6">
-        <v>0</v>
-      </c>
-      <c r="M26" t="s">
+      <c r="H29" s="17">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I29" s="17">
+        <v>8</v>
+      </c>
+      <c r="J29" s="6">
+        <v>0</v>
+      </c>
+      <c r="K29" s="6">
+        <v>0</v>
+      </c>
+      <c r="L29" s="6">
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>252</v>
+      </c>
+      <c r="O29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G30">
+        <v>0.75766</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I30" s="6">
+        <v>8</v>
+      </c>
+      <c r="J30" s="6">
+        <v>0</v>
+      </c>
+      <c r="K30" s="6">
+        <v>0</v>
+      </c>
+      <c r="L30" s="6">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
         <v>229</v>
       </c>
-      <c r="O26" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="6" t="s">
+      <c r="N30" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27">
-        <v>22</v>
-      </c>
-      <c r="D27" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31">
+        <v>0.2</v>
+      </c>
+      <c r="F31" s="6">
         <v>0.1</v>
       </c>
-      <c r="G27">
-        <v>0.75766</v>
-      </c>
-      <c r="H27" s="6">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I27" s="6">
-        <v>8</v>
-      </c>
-      <c r="J27" s="6">
-        <v>0</v>
-      </c>
-      <c r="K27" s="6">
-        <v>0</v>
-      </c>
-      <c r="L27" s="6">
-        <v>0</v>
-      </c>
-      <c r="N27" s="6">
-        <v>0.24</v>
-      </c>
-      <c r="O27" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28">
-        <v>30</v>
-      </c>
-      <c r="D28" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28">
+      <c r="G31">
+        <v>1.51532</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I31" s="6">
+        <v>8</v>
+      </c>
+      <c r="J31" s="6">
+        <v>0</v>
+      </c>
+      <c r="K31" s="6">
+        <v>0</v>
+      </c>
+      <c r="L31" s="6">
+        <v>0</v>
+      </c>
+      <c r="M31" t="s">
+        <v>229</v>
+      </c>
+      <c r="N31" s="6">
         <v>0.2</v>
       </c>
-      <c r="F28" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="G28">
-        <v>1.51532</v>
-      </c>
-      <c r="H28" s="6">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="I28" s="6">
-        <v>8</v>
-      </c>
-      <c r="J28" s="6">
-        <v>0</v>
-      </c>
-      <c r="K28" s="6">
-        <v>0</v>
-      </c>
-      <c r="L28" s="6">
-        <v>0</v>
-      </c>
-      <c r="N28" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="O28" s="8" t="s">
+      <c r="O31" s="8" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" t="s">
+        <v>240</v>
+      </c>
+      <c r="C32">
+        <v>2000</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>331.8</v>
+      </c>
+      <c r="H32" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I32" s="6">
+        <v>8</v>
+      </c>
+      <c r="J32" s="6">
+        <v>0</v>
+      </c>
+      <c r="K32" s="6">
+        <v>0</v>
+      </c>
+      <c r="L32" s="6">
+        <v>0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B33" t="s">
+        <v>241</v>
+      </c>
+      <c r="C33">
+        <v>5000</v>
+      </c>
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G33">
+        <v>829.5</v>
+      </c>
+      <c r="H33" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I33" s="6">
+        <v>8</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0</v>
+      </c>
+      <c r="K33" s="6">
+        <v>0</v>
+      </c>
+      <c r="L33" s="6">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B34" t="s">
+        <v>242</v>
+      </c>
+      <c r="C34">
+        <v>4000</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>0.05</v>
+      </c>
+      <c r="G34">
+        <v>663.6</v>
+      </c>
+      <c r="H34" s="6">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="I34" s="6">
+        <v>8</v>
+      </c>
+      <c r="J34" s="6">
+        <v>0</v>
+      </c>
+      <c r="K34" s="6">
+        <v>0</v>
+      </c>
+      <c r="L34" s="6">
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O27" r:id="rId1"/>
-    <hyperlink ref="O28" r:id="rId2"/>
+    <hyperlink ref="O30" r:id="rId1"/>
+    <hyperlink ref="O31" r:id="rId2"/>
+    <hyperlink ref="O13" r:id="rId3"/>
+    <hyperlink ref="O14" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2827,12 +3111,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.25" customHeight="1">
+    <row r="1" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2858,7 +3142,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1">
+    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2881,7 +3165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1">
+    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -2904,7 +3188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29" thickBot="1">
+    <row r="4" spans="1:8" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2929,11 +3213,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2945,9 +3224,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" thickBot="1">
+    <row r="1" spans="1:7" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2970,7 +3249,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2993,7 +3272,7 @@
         <v>2.9559999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -3018,11 +3297,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3034,13 +3308,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" thickBot="1">
+    <row r="1" spans="1:11" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3075,7 +3349,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3112,11 +3386,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3128,9 +3397,9 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="43" thickBot="1">
+    <row r="1" spans="1:13" ht="46" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3171,7 +3440,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" thickBot="1">
+    <row r="2" spans="1:13" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -3212,7 +3481,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -3255,11 +3524,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3271,9 +3535,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" thickBot="1">
+    <row r="1" spans="1:11" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3308,7 +3572,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -3343,7 +3607,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29" thickBot="1">
+    <row r="3" spans="1:11" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>165</v>
       </c>
@@ -3378,7 +3642,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1">
+    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>165</v>
       </c>
@@ -3415,11 +3679,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3431,14 +3690,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" thickBot="1">
+    <row r="1" spans="1:12" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3476,7 +3735,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -3514,7 +3773,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -3552,7 +3811,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -3590,7 +3849,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -3628,7 +3887,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -3666,7 +3925,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -3704,7 +3963,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -3742,7 +4001,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -3780,7 +4039,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -3818,7 +4077,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -3856,7 +4115,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -3900,11 +4159,6 @@
     <hyperlink ref="L10" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3916,9 +4170,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="29" thickBot="1">
+    <row r="1" spans="1:9" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3947,7 +4201,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -3976,7 +4230,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -4005,7 +4259,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -4033,10 +4287,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>